<commit_message>
git ignore file added
</commit_message>
<xml_diff>
--- a/media/excel_file/output.xlsx
+++ b/media/excel_file/output.xlsx
@@ -14,130 +14,58 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
-  <si>
-    <t>submit_date</t>
-  </si>
-  <si>
-    <t>modify_date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>father_husband_name</t>
-  </si>
-  <si>
-    <t>mother_name</t>
+    <t>image_url</t>
   </si>
   <si>
     <t>gender</t>
   </si>
   <si>
-    <t>dob</t>
-  </si>
-  <si>
-    <t>marital_status</t>
-  </si>
-  <si>
-    <t>education</t>
-  </si>
-  <si>
-    <t>education_status</t>
-  </si>
-  <si>
-    <t>occupation</t>
-  </si>
-  <si>
-    <t>occupation_description</t>
-  </si>
-  <si>
     <t>mobile</t>
   </si>
   <si>
-    <t>flat_room_block_no</t>
-  </si>
-  <si>
-    <t>premises_building_villa</t>
-  </si>
-  <si>
-    <t>road_street_lane</t>
-  </si>
-  <si>
-    <t>area_locality_taluk</t>
-  </si>
-  <si>
-    <t>pin_code</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>district</t>
-  </si>
-  <si>
-    <t>2019-11-15</t>
-  </si>
-  <si>
-    <t>Ataulla</t>
-  </si>
-  <si>
-    <t>ibhhibhib</t>
-  </si>
-  <si>
-    <t>nasim</t>
+    <t>address</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>/home/arima/Music/jivan_jyoti/media/_DSC0103_j2HKMEm.JPG</t>
+  </si>
+  <si>
+    <t>/home/arima/Music/jivan_jyoti/media/_DSC0103_NMzsSLu.JPG</t>
+  </si>
+  <si>
+    <t>/home/arima/Music/jivan_jyoti/media/_DSC0103_Si6HLpy.JPG</t>
+  </si>
+  <si>
+    <t>http://35.224.167.35/media/_DSC0103_DR3e4ES.JPG</t>
   </si>
   <si>
     <t>male</t>
   </si>
   <si>
-    <t>1994-08-13</t>
-  </si>
-  <si>
-    <t>single</t>
-  </si>
-  <si>
-    <t>MCA</t>
-  </si>
-  <si>
-    <t>Complited</t>
-  </si>
-  <si>
-    <t>Private Job</t>
-  </si>
-  <si>
-    <t>developer</t>
-  </si>
-  <si>
-    <t>9515387817</t>
-  </si>
-  <si>
-    <t>153</t>
-  </si>
-  <si>
-    <t>krishna nivas</t>
-  </si>
-  <si>
-    <t>mico layout</t>
-  </si>
-  <si>
-    <t>hongsandra</t>
-  </si>
-  <si>
-    <t>500106</t>
-  </si>
-  <si>
-    <t>karnatka</t>
+    <t>9515387815</t>
   </si>
   <si>
     <t>banglore</t>
+  </si>
+  <si>
+    <t>kafksdfdfsf</t>
+  </si>
+  <si>
+    <t>kafksdfdfsfhff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +80,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,16 +121,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -488,13 +429,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,118 +451,91 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>20</v>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" t="s">
-        <v>37</v>
-      </c>
-      <c r="U2" t="s">
-        <v>38</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>